<commit_message>
Database helper added. Utilities added.
</commit_message>
<xml_diff>
--- a/DataBaseMoneyIO.xlsx
+++ b/DataBaseMoneyIO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DataBase" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>price</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>(in/out)</t>
   </si>
 </sst>
 </file>
@@ -498,29 +504,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D3"/>
+  <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
@@ -528,7 +537,15 @@
         <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -540,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B7:B8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Alarm fragment added for test. Notification method added in Utilities. Quit and logout btns are working. OnBackPressed overrided everywhere. Added checks to strings. And more...
</commit_message>
<xml_diff>
--- a/DataBaseMoneyIO.xlsx
+++ b/DataBaseMoneyIO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>price</t>
   </si>
@@ -115,13 +115,16 @@
     <t>picture ID</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
     <t>(in/out)</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Integer</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +510,7 @@
   <dimension ref="B2:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +523,7 @@
         <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -534,18 +537,18 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>